<commit_message>
función para ejecutar todas las instancias con los solver
</commit_message>
<xml_diff>
--- a/data/inst_9_dia_3.xlsx
+++ b/data/inst_9_dia_3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flexible-vrp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartaSierra\PycharmProjects\flexible-vrp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F588E33B-0F83-498B-929E-FAA03C89EE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95510442-6805-4367-83C0-271637B33231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,19 +18,6 @@
     <sheet name="comp_quantity_inst1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -555,7 +542,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -665,7 +652,8 @@
         <v>28</v>
       </c>
       <c r="B13">
-        <v>135</v>
+        <f>SUM(comp_quantity_inst1!C2:C20)</f>
+        <v>610</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -673,6 +661,7 @@
         <v>29</v>
       </c>
       <c r="B14">
+        <f>SUM(comp_quantity_inst1!C21:C34)</f>
         <v>3300</v>
       </c>
     </row>
@@ -1332,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D34" sqref="A1:D34"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>